<commit_message>
Repository cloned to local machine and executed succesfully.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arjun.shenoy\Documents\UiPath\IPLMatchDetails2021\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arjun.shenoy\Documents\UiPath\UIPATHAutomationClone_001\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8047F627-922A-46BC-8FB4-E177CB641D42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F52F6E8-922A-4901-B293-4A28C60CA8BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -177,7 +177,7 @@
     <t>https://www.cricbuzz.com</t>
   </si>
   <si>
-    <t>Data\Output\IPLData2021.xlsx</t>
+    <t>Data\Output\IPLData2021[cloned].xlsx</t>
   </si>
 </sst>
 </file>
@@ -557,7 +557,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>